<commit_message>
updated timesheets for 3/9
</commit_message>
<xml_diff>
--- a/Admin/Ara Folder/Spring Semester/Timesheet_2-27_3-5.xlsx
+++ b/Admin/Ara Folder/Spring Semester/Timesheet_2-27_3-5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borde\Senior Design Project\Admin\Ara Folder\Spring Semester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0EDE53-7C27-4694-8468-2D95BC21BF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A2F8B4-8F77-4332-B2E3-481397A43C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1BC5497-AAD9-4DDC-8628-751A33E9D351}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,11 +771,13 @@
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="G13" s="8">
+        <v>2</v>
+      </c>
       <c r="H13" s="9"/>
       <c r="I13" s="10">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -834,7 +836,7 @@
       </c>
       <c r="G16" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H16" s="10">
         <f t="shared" si="1"/>
@@ -842,7 +844,7 @@
       </c>
       <c r="I16" s="10">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>